<commit_message>
bugs on evaluation object solved
</commit_message>
<xml_diff>
--- a/assets/docs/Reporte_Anual.xlsx
+++ b/assets/docs/Reporte_Anual.xlsx
@@ -42,7 +42,7 @@
     <t>Responsabilidades</t>
   </si>
   <si>
-    <t>Promedio</t>
+    <t>Resultado</t>
   </si>
   <si>
     <t>Rating 2012</t>
@@ -1625,7 +1625,7 @@
     <col min="6" max="6" width="40" customWidth="true" style="0"/>
     <col min="7" max="7" width="16.138916" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="22.423096" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="11.140137" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="12.425537" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="14.853516" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="14.853516" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="14.853516" bestFit="true" customWidth="true" style="0"/>

</xml_diff>